<commit_message>
thay đổi form và trang import
</commit_message>
<xml_diff>
--- a/assets/uploads/templates/MauDuLieu_nhacungcap.xlsx
+++ b/assets/uploads/templates/MauDuLieu_nhacungcap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ncc_code</t>
   </si>
@@ -69,6 +69,27 @@
   </si>
   <si>
     <t>Đây là nhà cung cấp Apple</t>
+  </si>
+  <si>
+    <t>ncc_anh</t>
+  </si>
+  <si>
+    <t>ncc_ngaytao</t>
+  </si>
+  <si>
+    <t>ncc_ngaycapnhat</t>
+  </si>
+  <si>
+    <t>/suppliers/anh1</t>
+  </si>
+  <si>
+    <t>/suppliers/anh2</t>
+  </si>
+  <si>
+    <t>/suppliers/anh3</t>
+  </si>
+  <si>
+    <t>/suppliers/anh4</t>
   </si>
 </sst>
 </file>
@@ -386,18 +407,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,8 +431,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -418,8 +451,11 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -429,8 +465,11 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -440,8 +479,11 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -450,6 +492,9 @@
       </c>
       <c r="C5" t="s">
         <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
thay đổi đường dẫn import ảnh
</commit_message>
<xml_diff>
--- a/assets/uploads/templates/MauDuLieu_nhacungcap.xlsx
+++ b/assets/uploads/templates/MauDuLieu_nhacungcap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>ncc_code</t>
   </si>
@@ -80,16 +80,7 @@
     <t>ncc_ngaycapnhat</t>
   </si>
   <si>
-    <t>/suppliers/anh1</t>
-  </si>
-  <si>
-    <t>/suppliers/anh2</t>
-  </si>
-  <si>
-    <t>/suppliers/anh3</t>
-  </si>
-  <si>
-    <t>/suppliers/anh4</t>
+    <t>Samsung.jpg</t>
   </si>
 </sst>
 </file>
@@ -410,7 +401,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +457,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -480,7 +471,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -494,7 +485,7 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/kellyfire611/onsite-web-job"
This reverts commit 93d4e17e94b0d088d3faa46fea729514137598cf, reversing
changes made to cf5e995f41720a157c6efe0a8e1aaeacee564151.
</commit_message>
<xml_diff>
--- a/assets/uploads/templates/MauDuLieu_nhacungcap.xlsx
+++ b/assets/uploads/templates/MauDuLieu_nhacungcap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ncc_code</t>
   </si>
@@ -80,7 +80,16 @@
     <t>ncc_ngaycapnhat</t>
   </si>
   <si>
-    <t>Samsung.jpg</t>
+    <t>/suppliers/anh1</t>
+  </si>
+  <si>
+    <t>/suppliers/anh2</t>
+  </si>
+  <si>
+    <t>/suppliers/anh3</t>
+  </si>
+  <si>
+    <t>/suppliers/anh4</t>
   </si>
 </sst>
 </file>
@@ -401,7 +410,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +466,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -471,7 +480,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -485,7 +494,7 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>